<commit_message>
creating dictionaries for each product
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
   <si>
     <t xml:space="preserve">product</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">iphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samsung</t>
   </si>
 </sst>
 </file>
@@ -135,7 +138,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,7 +255,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>972</v>
@@ -340,7 +343,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>908</v>

</xml_diff>

<commit_message>
showing the user product and calculations + fixing a bug in making dictionaries for products
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -50,6 +50,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -109,8 +110,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -138,240 +143,240 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>44562</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>914</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>44593</v>
+      <c r="C3" s="2" t="n">
+        <v>44563</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>902</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>44621</v>
+      <c r="C4" s="2" t="n">
+        <v>44564</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>904</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>44652</v>
+      <c r="C5" s="2" t="n">
+        <v>44565</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>1066</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>44682</v>
+      <c r="C6" s="2" t="n">
+        <v>44566</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>1017</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>44713</v>
+      <c r="C7" s="2" t="n">
+        <v>44567</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>930</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>44743</v>
+      <c r="C8" s="2" t="n">
+        <v>44568</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>955</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>44774</v>
+      <c r="C9" s="2" t="n">
+        <v>44569</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>1055</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>44805</v>
+      <c r="C10" s="2" t="n">
+        <v>44570</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>972</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>44835</v>
+      <c r="C11" s="2" t="n">
+        <v>44571</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>971</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>44866</v>
+      <c r="C12" s="2" t="n">
+        <v>44572</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>1082</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>44896</v>
+      <c r="C13" s="2" t="n">
+        <v>44573</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>1017</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>44927</v>
+      <c r="C14" s="2" t="n">
+        <v>44574</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>969</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>44958</v>
+      <c r="C15" s="2" t="n">
+        <v>44575</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="0" t="n">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>952</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>44986</v>
+      <c r="C16" s="2" t="n">
+        <v>44576</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="0" t="n">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>1094</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>45017</v>
+      <c r="C17" s="2" t="n">
+        <v>44577</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="0" t="n">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>971</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>45047</v>
+      <c r="C18" s="2" t="n">
+        <v>44578</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>908</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>45078</v>
+      <c r="C19" s="2" t="n">
+        <v>44579</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>960</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>45108</v>
+      <c r="C20" s="2" t="n">
+        <v>44580</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="0" t="n">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1" t="n">
         <v>921</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>45139</v>
+      <c r="C21" s="2" t="n">
+        <v>44579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
total average price has been added
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
   <si>
     <t xml:space="preserve">product</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">samsung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xiaomi</t>
   </si>
 </sst>
 </file>
@@ -140,13 +143,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -377,6 +380,50 @@
       </c>
       <c r="C21" s="2" t="n">
         <v>44579</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>802</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>800</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>44563</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>44564</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>740</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>44565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>